<commit_message>
The script for obtaining data from the table is ready as a whole, it remains to finish the little things, but everything works
</commit_message>
<xml_diff>
--- a/src/data/table.xlsx
+++ b/src/data/table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shiva\Documents\hmel-and-coffee\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA9152B-7ECC-4F4E-A1A1-38DB4DB62A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EBC080-431E-4591-9991-31144909E3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{B42A3BA8-976A-43A9-8DC6-1FA0F0B929D7}"/>
+    <workbookView xWindow="2730" yWindow="2985" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{B42A3BA8-976A-43A9-8DC6-1FA0F0B929D7}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="1" r:id="rId1"/>
@@ -190,6 +190,9 @@
     <t>--</t>
   </si>
   <si>
+    <t>+</t>
+  </si>
+  <si>
     <t>Somnambula</t>
   </si>
   <si>
@@ -225,9 +228,6 @@
   <si>
     <t>Sour-Smoothie 
 /Pastry</t>
-  </si>
-  <si>
-    <t>+</t>
   </si>
 </sst>
 </file>
@@ -284,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -296,6 +296,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1208,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E946BA-2947-4932-BA25-9C916E7062DF}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A535" workbookViewId="0">
-      <selection activeCell="A560" sqref="A560"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="A1:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,7 +1229,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>34</v>
@@ -1254,7 +1258,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>38</v>
@@ -1283,7 +1287,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>41</v>
@@ -1312,7 +1316,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>43</v>
@@ -1341,7 +1345,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>46</v>
@@ -1369,149 +1373,36 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="4">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="4">
-        <v>22</v>
-      </c>
-      <c r="H6" s="4">
-        <v>20</v>
-      </c>
-      <c r="I6" s="4">
-        <v>298</v>
-      </c>
+      <c r="C6" s="7"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="7"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="4">
-        <v>5</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="4">
-        <v>12.5</v>
-      </c>
-      <c r="I7" s="4">
-        <v>388</v>
-      </c>
+      <c r="C7" s="7"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="6"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="4">
-        <v>6</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="4">
-        <v>16</v>
-      </c>
-      <c r="I8" s="4">
-        <v>270</v>
-      </c>
+      <c r="C8" s="7"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="4">
-        <v>6</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="4">
-        <v>23</v>
-      </c>
-      <c r="H9" s="4">
-        <v>17</v>
-      </c>
-      <c r="I9" s="4">
-        <v>314</v>
-      </c>
+      <c r="C9" s="7"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="7"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="4">
-        <v>6</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="4">
-        <v>20</v>
-      </c>
-      <c r="H10" s="4">
-        <v>21</v>
-      </c>
-      <c r="I10" s="4">
-        <v>292</v>
-      </c>
+      <c r="C10" s="7"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="7"/>
+      <c r="I10" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1533,23 +1424,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7E27D-EAD8-4FA3-B941-64B2DA06036C}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1557,32 +1448,152 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="9">
+        <v>8</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="9">
+        <v>22</v>
+      </c>
+      <c r="O3" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="9">
+        <v>5</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" s="9">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="9">
+        <v>6</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="9">
+        <v>6</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" s="9">
+        <v>23</v>
+      </c>
+      <c r="O6" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="9">
+        <v>6</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="9">
+        <v>20</v>
+      </c>
+      <c r="O7" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
the script for obtaining data from the table for cards works completely, all that remains is to write a script to obtain data for the table
</commit_message>
<xml_diff>
--- a/src/data/table.xlsx
+++ b/src/data/table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shiva\Documents\hmel-and-coffee\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EBC080-431E-4591-9991-31144909E3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF70E4E6-5940-4078-A244-7A3D5CD6DA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2985" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{B42A3BA8-976A-43A9-8DC6-1FA0F0B929D7}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{B42A3BA8-976A-43A9-8DC6-1FA0F0B929D7}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
   <si>
     <t>кран</t>
   </si>
@@ -228,6 +228,21 @@
   <si>
     <t>Sour-Smoothie 
 /Pastry</t>
+  </si>
+  <si>
+    <t>/src/img/png/product/somnambula.png</t>
+  </si>
+  <si>
+    <t>/src/img/png/product/new_england.png</t>
+  </si>
+  <si>
+    <t>/src/img/png/product/nitro.png</t>
+  </si>
+  <si>
+    <t>/src/img/png/product/stoner_milk.png</t>
+  </si>
+  <si>
+    <t>/src/img/png/product/tropical_slasher.png</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1228,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="A1:I5"/>
+      <selection activeCell="I5" sqref="I1:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,15 +1439,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7E27D-EAD8-4FA3-B941-64B2DA06036C}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:B2"/>
+      <selection activeCell="H3" sqref="H3:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1440,7 +1455,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1448,7 +1463,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1476,8 +1491,14 @@
       <c r="O3" s="9">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="9">
+        <v>334</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1505,8 +1526,14 @@
       <c r="O4" s="9">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="9">
+        <v>307</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1534,8 +1561,14 @@
       <c r="O5" s="9">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="9">
+        <v>249</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1563,8 +1596,14 @@
       <c r="O6" s="9">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="9">
+        <v>208</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1592,8 +1631,14 @@
       <c r="O7" s="9">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="9">
+        <v>368</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
all parsers are ready, only PC adaption remains
</commit_message>
<xml_diff>
--- a/src/data/table.xlsx
+++ b/src/data/table.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shiva\Documents\hmel-and-coffee\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8313493C-A289-42C0-8211-5840B4E9DD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2E1529-361D-4BFB-AB8F-A0CAF25C0552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B42A3BA8-976A-43A9-8DC6-1FA0F0B929D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{B42A3BA8-976A-43A9-8DC6-1FA0F0B929D7}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="1" r:id="rId1"/>
     <sheet name="card" sheetId="3" r:id="rId2"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId3"/>
+    <sheet name="poster" sheetId="4" r:id="rId3"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
   <si>
     <t>зимняя меланхолия</t>
   </si>
@@ -240,13 +241,19 @@
   </si>
   <si>
     <t>/src/img/png/product/mixtape.png</t>
+  </si>
+  <si>
+    <t>НХЛ Филадельфия-Бостон регулярный чемпионат 20:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НХЛ Бостон-Лос-Анджелес регулярный чемпионат 20:30 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +289,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -304,7 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -327,6 +341,11 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -644,7 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19314601-5097-4EC3-924C-C1EDBCB0C61E}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1287,6 +1306,91 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66956A95-FF35-4AC6-8FAF-E32F5CB534CF}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="20">
+        <v>44997</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="20">
+        <v>45028</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="20">
+        <v>45058</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="20">
+        <v>45058</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
+        <v>45119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="20">
+        <v>45150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
+        <v>45181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>45272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
+        <v>45374</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="20">
+        <v>45649</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>45669</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7E27D-EAD8-4FA3-B941-64B2DA06036C}">
   <dimension ref="A1:P8"/>
   <sheetViews>

</xml_diff>

<commit_message>
PC adaption started, host does not work
</commit_message>
<xml_diff>
--- a/src/data/table.xlsx
+++ b/src/data/table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shiva\Documents\hmel-and-coffee\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2E1529-361D-4BFB-AB8F-A0CAF25C0552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA67B99-CDD6-49C0-88B0-5CC87F7E327E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{B42A3BA8-976A-43A9-8DC6-1FA0F0B929D7}"/>
   </bookViews>
@@ -253,13 +253,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -316,15 +323,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -333,22 +340,23 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{1F3007DE-6951-4DEF-AFE1-6203BA188FA6}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -365,9 +373,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -405,7 +413,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -511,7 +519,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -664,7 +672,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,9 +863,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>8</v>
-      </c>
+      <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
@@ -907,7 +913,9 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
@@ -953,7 +961,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,8 +1008,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>44</v>
+      <c r="A2" s="23" t="s">
+        <v>27</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>32</v>
@@ -1288,7 +1296,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1310,7 +1318,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,7 +1378,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
-        <v>45649</v>
+        <v>45616</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>66</v>

</xml_diff>